<commit_message>
relative effectiveness and league tables are done (finallly). studies table is using DataTables now, so we can sort, search, hide columns and all that stuff
</commit_message>
<xml_diff>
--- a/data/NMA_Tool.xlsx
+++ b/data/NMA_Tool.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="NMA_Tool" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NMA_Tool!$N$1:$N$241</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1699,9 +1702,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -23954,6 +23965,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="N1:N241"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>